<commit_message>
DOCS: minor fix to demo of sternberg memory sets
a few of the entries had duplicate numbers in the memory sets
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/sternberg/mainTrials.xlsx
+++ b/psychopy/demos/builder/sternberg/mainTrials.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lpzjwp/code/psychopy/git/psychopy/demos/builder/sternberg/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F037E519-A7D4-3947-8E42-551B448D4177}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6840" yWindow="6120" windowWidth="25940" windowHeight="18780" tabRatio="500"/>
+    <workbookView xWindow="6840" yWindow="6120" windowWidth="25940" windowHeight="18780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130406" concurrentCalc="0"/>
+  <calcPr calcId="130406"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -19,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jon Peirce</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -432,15 +438,6 @@
     <t>7 1 8 4 9 3</t>
   </si>
   <si>
-    <t>3 4 9 6 2 9</t>
-  </si>
-  <si>
-    <t>5 7 8 2 3 8</t>
-  </si>
-  <si>
-    <t>6 8 9 3 4 9</t>
-  </si>
-  <si>
     <t>7 6 4 8 1 2</t>
   </si>
   <si>
@@ -451,13 +448,22 @@
   </si>
   <si>
     <t>right</t>
+  </si>
+  <si>
+    <t>3 4 9 6 2 5</t>
+  </si>
+  <si>
+    <t>5 7 8 2 3 4</t>
+  </si>
+  <si>
+    <t>6 8 9 3 4 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -508,6 +514,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -830,19 +844,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" style="1"/>
+    <col min="4" max="4" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -862,7 +876,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -879,10 +893,10 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -899,10 +913,10 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
@@ -919,10 +933,10 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1</v>
       </c>
@@ -939,10 +953,10 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1</v>
       </c>
@@ -959,10 +973,10 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1</v>
       </c>
@@ -979,10 +993,10 @@
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2</v>
       </c>
@@ -999,10 +1013,10 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1019,10 +1033,10 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1039,10 +1053,10 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1059,10 +1073,10 @@
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1079,10 +1093,10 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1099,10 +1113,10 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1119,10 +1133,10 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1139,10 +1153,10 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1159,10 +1173,10 @@
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1179,10 +1193,10 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1199,10 +1213,10 @@
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1219,10 +1233,10 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1239,10 +1253,10 @@
         <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1259,10 +1273,10 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1279,10 +1293,10 @@
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1299,10 +1313,10 @@
         <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1319,10 +1333,10 @@
         <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1339,10 +1353,10 @@
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
@@ -1359,10 +1373,10 @@
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1379,10 +1393,10 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1399,10 +1413,10 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>3</v>
       </c>
@@ -1419,10 +1433,10 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1439,10 +1453,10 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1459,10 +1473,10 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>3</v>
       </c>
@@ -1479,10 +1493,10 @@
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1499,10 +1513,10 @@
         <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1519,10 +1533,10 @@
         <v>8</v>
       </c>
       <c r="F34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1539,10 +1553,10 @@
         <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1559,10 +1573,10 @@
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>3</v>
       </c>
@@ -1579,10 +1593,10 @@
         <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>4</v>
       </c>
@@ -1599,10 +1613,10 @@
         <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>4</v>
       </c>
@@ -1619,10 +1633,10 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>4</v>
       </c>
@@ -1639,10 +1653,10 @@
         <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1659,10 +1673,10 @@
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>4</v>
       </c>
@@ -1679,10 +1693,10 @@
         <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>4</v>
       </c>
@@ -1699,10 +1713,10 @@
         <v>4</v>
       </c>
       <c r="F43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>4</v>
       </c>
@@ -1719,10 +1733,10 @@
         <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>4</v>
       </c>
@@ -1739,10 +1753,10 @@
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>4</v>
       </c>
@@ -1759,10 +1773,10 @@
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>4</v>
       </c>
@@ -1779,10 +1793,10 @@
         <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>4</v>
       </c>
@@ -1799,10 +1813,10 @@
         <v>9</v>
       </c>
       <c r="F48" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>4</v>
       </c>
@@ -1819,10 +1833,10 @@
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>4</v>
       </c>
@@ -1839,10 +1853,10 @@
         <v>3</v>
       </c>
       <c r="F50" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>4</v>
       </c>
@@ -1859,10 +1873,10 @@
         <v>5</v>
       </c>
       <c r="F51" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>4</v>
       </c>
@@ -1879,10 +1893,10 @@
         <v>6</v>
       </c>
       <c r="F52" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>4</v>
       </c>
@@ -1899,10 +1913,10 @@
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>4</v>
       </c>
@@ -1919,10 +1933,10 @@
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>4</v>
       </c>
@@ -1939,10 +1953,10 @@
         <v>7</v>
       </c>
       <c r="F55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>4</v>
       </c>
@@ -1959,10 +1973,10 @@
         <v>4</v>
       </c>
       <c r="F56" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>4</v>
       </c>
@@ -1979,10 +1993,10 @@
         <v>7</v>
       </c>
       <c r="F57" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>4</v>
       </c>
@@ -1999,10 +2013,10 @@
         <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>4</v>
       </c>
@@ -2019,10 +2033,10 @@
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>4</v>
       </c>
@@ -2039,10 +2053,10 @@
         <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>4</v>
       </c>
@@ -2059,10 +2073,10 @@
         <v>2</v>
       </c>
       <c r="F61" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>5</v>
       </c>
@@ -2079,10 +2093,10 @@
         <v>8</v>
       </c>
       <c r="F62" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>5</v>
       </c>
@@ -2099,10 +2113,10 @@
         <v>3</v>
       </c>
       <c r="F63" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>5</v>
       </c>
@@ -2119,10 +2133,10 @@
         <v>7</v>
       </c>
       <c r="F64" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>5</v>
       </c>
@@ -2139,10 +2153,10 @@
         <v>9</v>
       </c>
       <c r="F65" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>5</v>
       </c>
@@ -2159,10 +2173,10 @@
         <v>8</v>
       </c>
       <c r="F66" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>5</v>
       </c>
@@ -2179,10 +2193,10 @@
         <v>9</v>
       </c>
       <c r="F67" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>5</v>
       </c>
@@ -2199,10 +2213,10 @@
         <v>5</v>
       </c>
       <c r="F68" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>5</v>
       </c>
@@ -2219,10 +2233,10 @@
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>5</v>
       </c>
@@ -2239,10 +2253,10 @@
         <v>6</v>
       </c>
       <c r="F70" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>5</v>
       </c>
@@ -2259,10 +2273,10 @@
         <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>5</v>
       </c>
@@ -2279,10 +2293,10 @@
         <v>2</v>
       </c>
       <c r="F72" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>5</v>
       </c>
@@ -2299,10 +2313,10 @@
         <v>3</v>
       </c>
       <c r="F73" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>5</v>
       </c>
@@ -2319,10 +2333,10 @@
         <v>5</v>
       </c>
       <c r="F74" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>5</v>
       </c>
@@ -2339,10 +2353,10 @@
         <v>4</v>
       </c>
       <c r="F75" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>5</v>
       </c>
@@ -2359,10 +2373,10 @@
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>5</v>
       </c>
@@ -2379,10 +2393,10 @@
         <v>4</v>
       </c>
       <c r="F77" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>5</v>
       </c>
@@ -2399,10 +2413,10 @@
         <v>7</v>
       </c>
       <c r="F78" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>5</v>
       </c>
@@ -2419,10 +2433,10 @@
         <v>8</v>
       </c>
       <c r="F79" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>5</v>
       </c>
@@ -2439,10 +2453,10 @@
         <v>9</v>
       </c>
       <c r="F80" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>5</v>
       </c>
@@ -2459,10 +2473,10 @@
         <v>1</v>
       </c>
       <c r="F81" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>5</v>
       </c>
@@ -2479,10 +2493,10 @@
         <v>8</v>
       </c>
       <c r="F82" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>5</v>
       </c>
@@ -2499,10 +2513,10 @@
         <v>2</v>
       </c>
       <c r="F83" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>5</v>
       </c>
@@ -2519,10 +2533,10 @@
         <v>3</v>
       </c>
       <c r="F84" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>5</v>
       </c>
@@ -2539,10 +2553,10 @@
         <v>4</v>
       </c>
       <c r="F85" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>5</v>
       </c>
@@ -2559,10 +2573,10 @@
         <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>5</v>
       </c>
@@ -2579,10 +2593,10 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>5</v>
       </c>
@@ -2599,10 +2613,10 @@
         <v>5</v>
       </c>
       <c r="F88" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>5</v>
       </c>
@@ -2619,10 +2633,10 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>5</v>
       </c>
@@ -2639,10 +2653,10 @@
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>5</v>
       </c>
@@ -2659,10 +2673,10 @@
         <v>2</v>
       </c>
       <c r="F91" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>6</v>
       </c>
@@ -2679,10 +2693,10 @@
         <v>4</v>
       </c>
       <c r="F92" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>6</v>
       </c>
@@ -2699,10 +2713,10 @@
         <v>7</v>
       </c>
       <c r="F93" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>6</v>
       </c>
@@ -2719,10 +2733,10 @@
         <v>8</v>
       </c>
       <c r="F94" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>6</v>
       </c>
@@ -2739,10 +2753,10 @@
         <v>6</v>
       </c>
       <c r="F95" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>6</v>
       </c>
@@ -2759,10 +2773,10 @@
         <v>2</v>
       </c>
       <c r="F96" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>6</v>
       </c>
@@ -2779,10 +2793,10 @@
         <v>3</v>
       </c>
       <c r="F97" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>6</v>
       </c>
@@ -2799,10 +2813,10 @@
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>6</v>
       </c>
@@ -2819,10 +2833,10 @@
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>6</v>
       </c>
@@ -2839,10 +2853,10 @@
         <v>2</v>
       </c>
       <c r="F100" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>6</v>
       </c>
@@ -2859,10 +2873,10 @@
         <v>5</v>
       </c>
       <c r="F101" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>6</v>
       </c>
@@ -2879,10 +2893,10 @@
         <v>9</v>
       </c>
       <c r="F102" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>6</v>
       </c>
@@ -2899,10 +2913,10 @@
         <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>6</v>
       </c>
@@ -2919,10 +2933,10 @@
         <v>7</v>
       </c>
       <c r="F104" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>6</v>
       </c>
@@ -2939,10 +2953,10 @@
         <v>4</v>
       </c>
       <c r="F105" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>6</v>
       </c>
@@ -2959,10 +2973,10 @@
         <v>5</v>
       </c>
       <c r="F106" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>6</v>
       </c>
@@ -2979,10 +2993,10 @@
         <v>9</v>
       </c>
       <c r="F107" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>6</v>
       </c>
@@ -2999,10 +3013,10 @@
         <v>8</v>
       </c>
       <c r="F108" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>6</v>
       </c>
@@ -3019,10 +3033,10 @@
         <v>9</v>
       </c>
       <c r="F109" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>6</v>
       </c>
@@ -3039,10 +3053,10 @@
         <v>8</v>
       </c>
       <c r="F110" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>6</v>
       </c>
@@ -3059,10 +3073,10 @@
         <v>6</v>
       </c>
       <c r="F111" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>6</v>
       </c>
@@ -3079,10 +3093,10 @@
         <v>7</v>
       </c>
       <c r="F112" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>6</v>
       </c>
@@ -3099,10 +3113,10 @@
         <v>8</v>
       </c>
       <c r="F113" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>6</v>
       </c>
@@ -3119,10 +3133,10 @@
         <v>6</v>
       </c>
       <c r="F114" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>6</v>
       </c>
@@ -3139,10 +3153,10 @@
         <v>7</v>
       </c>
       <c r="F115" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>6</v>
       </c>
@@ -3159,10 +3173,10 @@
         <v>3</v>
       </c>
       <c r="F116" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A117">
         <v>6</v>
       </c>
@@ -3179,10 +3193,10 @@
         <v>5</v>
       </c>
       <c r="F117" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A118">
         <v>6</v>
       </c>
@@ -3199,90 +3213,90 @@
         <v>6</v>
       </c>
       <c r="F118" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A119">
+        <v>6</v>
+      </c>
+      <c r="B119">
+        <v>5</v>
+      </c>
+      <c r="C119" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E119">
+        <v>2</v>
+      </c>
+      <c r="F119" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A120">
+        <v>6</v>
+      </c>
+      <c r="B120">
+        <v>5</v>
+      </c>
+      <c r="C120" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119">
-        <v>6</v>
-      </c>
-      <c r="B119">
-        <v>5</v>
-      </c>
-      <c r="C119" t="s">
-        <v>11</v>
-      </c>
-      <c r="D119" s="1" t="s">
+      <c r="E120">
+        <v>3</v>
+      </c>
+      <c r="F120" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A121">
+        <v>6</v>
+      </c>
+      <c r="B121">
+        <v>5</v>
+      </c>
+      <c r="C121" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E121">
+        <v>4</v>
+      </c>
+      <c r="F121" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A122">
+        <v>6</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C122" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E119">
-        <v>2</v>
-      </c>
-      <c r="F119" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120">
-        <v>6</v>
-      </c>
-      <c r="B120">
-        <v>5</v>
-      </c>
-      <c r="C120" t="s">
-        <v>11</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E120">
-        <v>3</v>
-      </c>
-      <c r="F120" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121">
-        <v>6</v>
-      </c>
-      <c r="B121">
-        <v>5</v>
-      </c>
-      <c r="C121" t="s">
-        <v>11</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E121">
-        <v>4</v>
-      </c>
-      <c r="F121" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122">
-        <v>6</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C122" t="s">
-        <v>12</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="E122">
         <v>9</v>
       </c>
       <c r="F122" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A123">
         <v>6</v>
       </c>
@@ -3293,16 +3307,16 @@
         <v>12</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E123">
         <v>8</v>
       </c>
       <c r="F123" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A124">
         <v>6</v>
       </c>
@@ -3319,10 +3333,10 @@
         <v>9</v>
       </c>
       <c r="F124" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A125">
         <v>6</v>
       </c>
@@ -3339,10 +3353,10 @@
         <v>3</v>
       </c>
       <c r="F125" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A126">
         <v>6</v>
       </c>
@@ -3359,10 +3373,10 @@
         <v>5</v>
       </c>
       <c r="F126" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A127">
         <v>6</v>
       </c>
@@ -3379,7 +3393,7 @@
         <v>6</v>
       </c>
       <c r="F127" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>